<commit_message>
[ATUALIZAÇÃO IMPORTANTE] Refatoração Capítulo 2
</commit_message>
<xml_diff>
--- a/Tabelas/Checklist.xlsx
+++ b/Tabelas/Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giovanni\Desktop\Monografia-USP\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1F3013F-AECC-45E4-A32E-2134A80AA37B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35BE7B7-6B77-4C5A-95DB-2BED6AEC4039}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3A68BAB9-AAAB-447F-8DC7-7F04D125C60E}"/>
+    <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{3A68BAB9-AAAB-447F-8DC7-7F04D125C60E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>4.3 As boas práticas de comunicação (5 C's) foram utilizadas na especificação?</t>
   </si>
   <si>
-    <t>4.4 O entendimento está equalizado entre os responsáveis?</t>
-  </si>
-  <si>
     <t>4. Refinamento dos requisitos entre os responsáveis</t>
   </si>
   <si>
@@ -123,13 +120,16 @@
   </si>
   <si>
     <t>[Descrição do domínio do sistema, exemplo: Transferências Bancárias]</t>
+  </si>
+  <si>
+    <t>4.4 Os cenários escritos estão de acordo com os 14 fatores?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +160,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -175,7 +182,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -198,22 +205,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -533,7 +556,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,191 +567,191 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="51" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="51" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>25</v>
+      <c r="B25" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>